<commit_message>
Site updated: 2020-07-24 18:20:53
</commit_message>
<xml_diff>
--- a/data/totaltime (2).xlsx
+++ b/data/totaltime (2).xlsx
@@ -393,13 +393,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="B2" t="str">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C2" t="str">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>